<commit_message>
Further work on the demo transition figure.
</commit_message>
<xml_diff>
--- a/chapters/ch03-Population/datasets/Demographic Transition.xlsx
+++ b/chapters/ch03-Population/datasets/Demographic Transition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch03-Population/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C1B9B4-17BF-5441-9D62-EE85B0B8C924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFA82DF-8946-AA4B-85B7-F6B1B5D17802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -927,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201:D251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3749,6 +3749,706 @@
         <v>99.781580779108495</v>
       </c>
     </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C202">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D202">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C203">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D203">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C204">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D204">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C205">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D205">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C206">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D206">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C207">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D207">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C208">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D208">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C209">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D209">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C210">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D210">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C211">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D211">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C212">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D212">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C213">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D213">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C214">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D214">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C215">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D215">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C216">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D216">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C217">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D217">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C218">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D218">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C219">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D219">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C220">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D220">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>220</v>
+      </c>
+      <c r="B221">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C221">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D221">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>221</v>
+      </c>
+      <c r="B222">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C222">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D222">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>222</v>
+      </c>
+      <c r="B223">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C223">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D223">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>223</v>
+      </c>
+      <c r="B224">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C224">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D224">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>224</v>
+      </c>
+      <c r="B225">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C225">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D225">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>225</v>
+      </c>
+      <c r="B226">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C226">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D226">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>226</v>
+      </c>
+      <c r="B227">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C227">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D227">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>227</v>
+      </c>
+      <c r="B228">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C228">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D228">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>228</v>
+      </c>
+      <c r="B229">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C229">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D229">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A230">
+        <v>229</v>
+      </c>
+      <c r="B230">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C230">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D230">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A231">
+        <v>230</v>
+      </c>
+      <c r="B231">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C231">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D231">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A232">
+        <v>231</v>
+      </c>
+      <c r="B232">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C232">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D232">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A233">
+        <v>232</v>
+      </c>
+      <c r="B233">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C233">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D233">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C234">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D234">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C235">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D235">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C236">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D236">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C237">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D237">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C238">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D238">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C239">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D239">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C240">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D240">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C241">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D241">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C242">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D242">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C243">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D243">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C244">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D244">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C245">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D245">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C246">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D246">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C247">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D247">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C248">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D248">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C249">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D249">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C250">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D250">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251">
+        <v>8.8839854167789998</v>
+      </c>
+      <c r="C251">
+        <v>8.9292780144256092</v>
+      </c>
+      <c r="D251">
+        <v>99.781580779108495</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>